<commit_message>
Enhance pabi_utils export excel, to have subtotal
</commit_message>
<xml_diff>
--- a/pabi_trial_balance_extension/xlsx_template/gfmis.xlsx
+++ b/pabi_trial_balance_extension/xlsx_template/gfmis.xlsx
@@ -50,11 +50,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="#,###.00"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,12 +107,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -142,7 +137,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,10 +161,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -184,8 +175,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -196,43 +187,42 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -305,38 +295,35 @@
   <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="12.1174089068826"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.69230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="7.21862348178138"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="8.74089068825911"/>
-    <col collapsed="false" hidden="false" max="1020" min="7" style="2" width="32.3198380566802"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="32.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="35.748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="3" width="15.3036437246964"/>
+    <col collapsed="false" hidden="false" max="1020" min="7" style="2" width="34.6437246963563"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
@@ -1353,14 +1340,14 @@
       <c r="AMF2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
@@ -2376,59 +2363,67 @@
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
     </row>
-    <row r="5" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+    <row r="4" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="ALC4" s="2"/>
+      <c r="ALD4" s="2"/>
+      <c r="ALE4" s="2"/>
+      <c r="ALF4" s="2"/>
+      <c r="ALG4" s="2"/>
+      <c r="ALH4" s="2"/>
+      <c r="ALI4" s="2"/>
+      <c r="ALJ4" s="2"/>
+      <c r="ALK4" s="2"/>
+      <c r="ALL4" s="2"/>
+      <c r="ALM4" s="2"/>
+      <c r="ALN4" s="2"/>
+      <c r="ALO4" s="2"/>
+      <c r="ALP4" s="2"/>
+      <c r="ALQ4" s="2"/>
+      <c r="ALR4" s="2"/>
+      <c r="ALS4" s="2"/>
+      <c r="ALT4" s="2"/>
+      <c r="ALU4" s="2"/>
+      <c r="ALV4" s="2"/>
+      <c r="ALW4" s="2"/>
+      <c r="ALX4" s="2"/>
+      <c r="ALY4" s="2"/>
+      <c r="ALZ4" s="2"/>
+      <c r="AMA4" s="2"/>
+      <c r="AMB4" s="2"/>
+      <c r="AMC4" s="2"/>
+      <c r="AMD4" s="2"/>
+      <c r="AME4" s="2"/>
+      <c r="AMF4" s="2"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="ALC5" s="2"/>
-      <c r="ALD5" s="2"/>
-      <c r="ALE5" s="2"/>
-      <c r="ALF5" s="2"/>
-      <c r="ALG5" s="2"/>
-      <c r="ALH5" s="2"/>
-      <c r="ALI5" s="2"/>
-      <c r="ALJ5" s="2"/>
-      <c r="ALK5" s="2"/>
-      <c r="ALL5" s="2"/>
-      <c r="ALM5" s="2"/>
-      <c r="ALN5" s="2"/>
-      <c r="ALO5" s="2"/>
-      <c r="ALP5" s="2"/>
-      <c r="ALQ5" s="2"/>
-      <c r="ALR5" s="2"/>
-      <c r="ALS5" s="2"/>
-      <c r="ALT5" s="2"/>
-      <c r="ALU5" s="2"/>
-      <c r="ALV5" s="2"/>
-      <c r="ALW5" s="2"/>
-      <c r="ALX5" s="2"/>
-      <c r="ALY5" s="2"/>
-      <c r="ALZ5" s="2"/>
-      <c r="AMA5" s="2"/>
-      <c r="AMB5" s="2"/>
-      <c r="AMC5" s="2"/>
-      <c r="AMD5" s="2"/>
-      <c r="AME5" s="2"/>
-      <c r="AMF5" s="2"/>
-      <c r="AMG5" s="0"/>
-      <c r="AMH5" s="0"/>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[ENH] trial balance for GFMIS
</commit_message>
<xml_diff>
--- a/pabi_trial_balance_extension/xlsx_template/gfmis.xlsx
+++ b/pabi_trial_balance_extension/xlsx_template/gfmis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Special Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Trial Balance for GFMIS</t>
   </si>
@@ -28,22 +28,40 @@
     <t xml:space="preserve">Fiscal Year:</t>
   </si>
   <si>
-    <t xml:space="preserve">Account Code</t>
+    <t xml:space="preserve">PABI2 A/C</t>
   </si>
   <si>
-    <t xml:space="preserve">Account Name</t>
+    <t xml:space="preserve">PABI2 A/C Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Initial</t>
+    <t xml:space="preserve">GFMIS A/C</t>
   </si>
   <si>
-    <t xml:space="preserve">Debit</t>
+    <t xml:space="preserve">GFMIS A/C Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Credit</t>
+    <t xml:space="preserve">Prev Bal – Debit</t>
   </si>
   <si>
-    <t xml:space="preserve">Balance</t>
+    <t xml:space="preserve">Prev Bal – Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving – Debit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving – Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving Bal – Debit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving Bal – Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Bal – Debit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Bal – Credit</t>
   </si>
 </sst>
 </file>
@@ -52,10 +70,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,###.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,6 +124,13 @@
       <name val="DejaVu Serif"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -162,7 +187,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +237,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,19 +321,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="35.748987854251"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="3" width="15.3036437246964"/>
-    <col collapsed="false" hidden="false" max="1020" min="7" style="2" width="34.6437246963563"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="8.81376518218623"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="5" style="3" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="2" width="34.64"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -312,24 +341,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
-      <c r="L2" s="0"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
       <c r="O2" s="0"/>
@@ -1338,22 +1373,26 @@
       <c r="AMD2" s="0"/>
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="0"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
-      <c r="K3" s="0"/>
-      <c r="L3" s="0"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
       <c r="O3" s="0"/>
@@ -2362,19 +2401,24 @@
       <c r="AMD3" s="0"/>
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="ALC4" s="2"/>
-      <c r="ALD4" s="2"/>
-      <c r="ALE4" s="2"/>
-      <c r="ALF4" s="2"/>
-      <c r="ALG4" s="2"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
       <c r="ALH4" s="2"/>
       <c r="ALI4" s="2"/>
       <c r="ALJ4" s="2"/>
@@ -2400,10 +2444,10 @@
       <c r="AMD4" s="2"/>
       <c r="AME4" s="2"/>
       <c r="AMF4" s="2"/>
-      <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
+      <c r="AMG4" s="2"/>
+      <c r="AMH4" s="2"/>
+      <c r="AMI4" s="2"/>
+      <c r="AMJ4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
@@ -2412,10 +2456,10 @@
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -2424,11 +2468,29 @@
       <c r="F5" s="12" t="s">
         <v>7</v>
       </c>
+      <c r="G5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[IMP] Add more reports
</commit_message>
<xml_diff>
--- a/pabi_trial_balance_extension/xlsx_template/gfmis.xlsx
+++ b/pabi_trial_balance_extension/xlsx_template/gfmis.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Trial Balance for GFMIS</t>
   </si>
   <si>
     <t xml:space="preserve">Fiscal Year:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PABI2 A/C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PABI2 A/C Name</t>
   </si>
   <si>
     <t xml:space="preserve">GFMIS A/C</t>
@@ -73,7 +67,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -98,12 +92,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="DejaVu Serif"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Serif"/>
       <family val="1"/>
@@ -115,7 +103,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -131,6 +118,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -187,7 +175,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,15 +184,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,23 +208,23 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,47 +308,46 @@
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="5" style="3" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="2" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="2" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="1" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="34.64"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="6" customFormat="true" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
       <c r="O2" s="0"/>
@@ -1375,24 +1358,22 @@
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
       <c r="O3" s="0"/>
@@ -2403,57 +2384,55 @@
       <c r="AMF3" s="0"/>
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="ALH4" s="2"/>
-      <c r="ALI4" s="2"/>
-      <c r="ALJ4" s="2"/>
-      <c r="ALK4" s="2"/>
-      <c r="ALL4" s="2"/>
-      <c r="ALM4" s="2"/>
-      <c r="ALN4" s="2"/>
-      <c r="ALO4" s="2"/>
-      <c r="ALP4" s="2"/>
-      <c r="ALQ4" s="2"/>
-      <c r="ALR4" s="2"/>
-      <c r="ALS4" s="2"/>
-      <c r="ALT4" s="2"/>
-      <c r="ALU4" s="2"/>
-      <c r="ALV4" s="2"/>
-      <c r="ALW4" s="2"/>
-      <c r="ALX4" s="2"/>
-      <c r="ALY4" s="2"/>
-      <c r="ALZ4" s="2"/>
-      <c r="AMA4" s="2"/>
-      <c r="AMB4" s="2"/>
-      <c r="AMC4" s="2"/>
-      <c r="AMD4" s="2"/>
-      <c r="AME4" s="2"/>
-      <c r="AMF4" s="2"/>
-      <c r="AMG4" s="2"/>
-      <c r="AMH4" s="2"/>
-      <c r="AMI4" s="2"/>
-      <c r="AMJ4" s="2"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="ALF4" s="1"/>
+      <c r="ALG4" s="1"/>
+      <c r="ALH4" s="1"/>
+      <c r="ALI4" s="1"/>
+      <c r="ALJ4" s="1"/>
+      <c r="ALK4" s="1"/>
+      <c r="ALL4" s="1"/>
+      <c r="ALM4" s="1"/>
+      <c r="ALN4" s="1"/>
+      <c r="ALO4" s="1"/>
+      <c r="ALP4" s="1"/>
+      <c r="ALQ4" s="1"/>
+      <c r="ALR4" s="1"/>
+      <c r="ALS4" s="1"/>
+      <c r="ALT4" s="1"/>
+      <c r="ALU4" s="1"/>
+      <c r="ALV4" s="1"/>
+      <c r="ALW4" s="1"/>
+      <c r="ALX4" s="1"/>
+      <c r="ALY4" s="1"/>
+      <c r="ALZ4" s="1"/>
+      <c r="AMA4" s="1"/>
+      <c r="AMB4" s="1"/>
+      <c r="AMC4" s="1"/>
+      <c r="AMD4" s="1"/>
+      <c r="AME4" s="1"/>
+      <c r="AMF4" s="1"/>
+      <c r="AMG4" s="1"/>
+      <c r="AMH4" s="1"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -2468,23 +2447,17 @@
       <c r="F5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>